<commit_message>
Changes on the final LCA report and presentation
</commit_message>
<xml_diff>
--- a/LCA/lca_comparison.xlsx
+++ b/LCA/lca_comparison.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="77">
   <si>
     <t xml:space="preserve">Functional unit</t>
   </si>
@@ -233,23 +233,44 @@
     <t xml:space="preserve">Total f.u.</t>
   </si>
   <si>
+    <t xml:space="preserve">Petrelaic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worst Biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Usage (m^3/fu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Demand (MJ/fu)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eutrophication potential (kg PO4 eq./f.u.) </t>
   </si>
   <si>
     <t xml:space="preserve">Human toxicity potential (kg DCB eq./f.u.) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.380</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="0"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -441,11 +462,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -604,205 +620,233 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -883,7 +927,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
@@ -938,8 +982,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.345917236635971"/>
-          <c:y val="0.0230411397005379"/>
+          <c:x val="0.345867247506592"/>
+          <c:y val="0.0230444896772318"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -957,10 +1001,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.129418058155974"/>
-          <c:y val="0.226922517807821"/>
-          <c:w val="0.844178671048107"/>
-          <c:h val="0.653801424625672"/>
+          <c:x val="0.12942794910008"/>
+          <c:y val="0.226955510322768"/>
+          <c:w val="0.844090335893615"/>
+          <c:h val="0.653751090433266"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1353,11 +1397,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="77530162"/>
-        <c:axId val="15096584"/>
+        <c:axId val="63715303"/>
+        <c:axId val="82318877"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77530162"/>
+        <c:axId val="63715303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1390,7 +1434,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15096584"/>
+        <c:crossAx val="82318877"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1398,7 +1442,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15096584"/>
+        <c:axId val="82318877"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1446,8 +1490,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.00683963165335677"/>
-              <c:y val="0.182584678005524"/>
+              <c:x val="0.00676372807520349"/>
+              <c:y val="0.18232044198895"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1485,7 +1529,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77530162"/>
+        <c:crossAx val="63715303"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1555,6 +1599,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.172306155574978"/>
+          <c:y val="0.0418789396425179"/>
+          <c:w val="0.678673991759271"/>
+          <c:h val="0.512390985234436"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1576,6 +1631,106 @@
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet5!$A$9:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Carbon footprint (kg CO2 eq./f.u.)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Water Usage (m^3/fu)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Energy Demand (MJ/fu)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Eutrophication potential (kg PO4 eq./f.u.) </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Human toxicity potential (kg DCB eq./f.u.) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$B$9:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>worst_biomass</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>worst_biomass</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
             </a:solidFill>
             <a:ln w="0">
               <a:noFill/>
@@ -1609,55 +1764,55 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$8:$A$13</c:f>
+              <c:f>Sheet5!$A$9:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Carbon footprint (kg CO2 eq./f.u.)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Acidification potential (kg SO2 eq./f.u.)</c:v>
+                  <c:v>Water Usage (m^3/fu)</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Energy Demand (MJ/fu)</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Eutrophication potential (kg PO4 eq./f.u.) </c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Human toxicity potential (kg DCB eq./f.u.) </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$B$8:$B$11</c:f>
+              <c:f>Sheet5!$D$9:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.00910189982728843</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.645</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.136159779614325</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.391666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0200714285714286</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>biomass</c:f>
@@ -1685,11 +1840,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1705,47 +1864,47 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$8:$A$13</c:f>
+              <c:f>Sheet5!$A$9:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Carbon footprint (kg CO2 eq./f.u.)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Acidification potential (kg SO2 eq./f.u.)</c:v>
+                  <c:v>Water Usage (m^3/fu)</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Energy Demand (MJ/fu)</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Eutrophication potential (kg PO4 eq./f.u.) </c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Human toxicity potential (kg DCB eq./f.u.) </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$C$8:$C$11</c:f>
+              <c:f>Sheet5!$C$9:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0089119170984456</c:v>
+                  <c:v>0.00639032815198618</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.037</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0150333333333333</c:v>
+                  <c:v>0.093939393939394</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0111785714285714</c:v>
+                  <c:v>0.283333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0135714285714286</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1753,17 +1912,17 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="70872062"/>
-        <c:axId val="33985145"/>
+        <c:axId val="82240325"/>
+        <c:axId val="80597424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70872062"/>
+        <c:axId val="82240325"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1780,12 +1939,15 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33985145"/>
+        <c:crossAx val="80597424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1793,7 +1955,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="33985145"/>
+        <c:axId val="80597424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1808,7 +1970,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1825,12 +1987,15 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70872062"/>
+        <c:crossAx val="82240325"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1845,6 +2010,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.806143472560405"/>
+          <c:y val="0.649568221070812"/>
+          <c:w val="0.183055503527502"/>
+          <c:h val="0.286614853195164"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1858,6 +2033,9 @@
         <a:p>
           <a:pPr>
             <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
@@ -1915,8 +2093,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.304677951035224"/>
-          <c:y val="0.0249076822822388"/>
+          <c:x val="0.304626439974812"/>
+          <c:y val="0.0249112897385763"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1934,10 +2112,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0939294047927701"/>
-          <c:y val="0.239446817753964"/>
-          <c:w val="0.8716619134042"/>
-          <c:h val="0.423358192744914"/>
+          <c:x val="0.0939363632996259"/>
+          <c:y val="0.239481497574046"/>
+          <c:w val="0.871578323517428"/>
+          <c:h val="0.423274675935984"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2474,11 +2652,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="32041481"/>
-        <c:axId val="57642357"/>
+        <c:axId val="34818668"/>
+        <c:axId val="46611197"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="32041481"/>
+        <c:axId val="34818668"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2511,7 +2689,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57642357"/>
+        <c:crossAx val="46611197"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2519,7 +2697,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57642357"/>
+        <c:axId val="46611197"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2567,8 +2745,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0114448683284566"/>
-              <c:y val="0.151256245022084"/>
+              <c:x val="0.0113716338852465"/>
+              <c:y val="0.15098848577015"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2606,7 +2784,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32041481"/>
+        <c:crossAx val="34818668"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2706,8 +2884,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.312673414357732"/>
-          <c:y val="0.0288364118151352"/>
+          <c:x val="0.312697854379177"/>
+          <c:y val="0.0288409073193546"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2725,10 +2903,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0405643049747939"/>
-          <c:y val="0.237082066869301"/>
-          <c:w val="0.958185157684943"/>
-          <c:h val="0.670017925337074"/>
+          <c:x val="0.0405674756712393"/>
+          <c:y val="0.237119027203991"/>
+          <c:w val="0.958103724547622"/>
+          <c:h val="0.669966482188791"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3103,11 +3281,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="47148821"/>
-        <c:axId val="95298219"/>
+        <c:axId val="44509751"/>
+        <c:axId val="68255012"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="47148821"/>
+        <c:axId val="44509751"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3140,7 +3318,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95298219"/>
+        <c:crossAx val="68255012"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3148,7 +3326,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95298219"/>
+        <c:axId val="68255012"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3191,7 +3369,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47148821"/>
+        <c:crossAx val="44509751"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3291,8 +3469,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.241619674185464"/>
-          <c:y val="0.0307334496220616"/>
+          <c:x val="0.241638599514373"/>
+          <c:y val="0.0307385561186342"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3310,10 +3488,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.06218671679198"/>
-          <c:y val="0.241714428108647"/>
-          <c:w val="0.91983865914787"/>
-          <c:h val="0.426364315973088"/>
+          <c:x val="0.0621915876870056"/>
+          <c:y val="0.241754590014123"/>
+          <c:w val="0.919754053418971"/>
+          <c:h val="0.426269003904627"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3814,11 +3992,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="35522991"/>
-        <c:axId val="78455330"/>
+        <c:axId val="96180249"/>
+        <c:axId val="32745407"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="35522991"/>
+        <c:axId val="96180249"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3851,7 +4029,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78455330"/>
+        <c:crossAx val="32745407"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3859,7 +4037,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78455330"/>
+        <c:axId val="32745407"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3902,7 +4080,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35522991"/>
+        <c:crossAx val="96180249"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4002,8 +4180,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.26326105598432"/>
-          <c:y val="0.0298578199052133"/>
+          <c:x val="0.263200882100707"/>
+          <c:y val="0.0298613579808034"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4021,10 +4199,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.100494099391564"/>
-          <c:y val="0.225355450236967"/>
-          <c:w val="0.873739229858304"/>
-          <c:h val="0.571149289099526"/>
+          <c:x val="0.100502307346755"/>
+          <c:y val="0.225382154283683"/>
+          <c:w val="0.873647241393392"/>
+          <c:h val="0.571098471382865"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -4339,11 +4517,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="4343859"/>
-        <c:axId val="1568728"/>
+        <c:axId val="74032005"/>
+        <c:axId val="99356174"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="4343859"/>
+        <c:axId val="74032005"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4381,8 +4559,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.319612887418841"/>
-              <c:y val="0.894372037914692"/>
+              <c:x val="0.319638992118267"/>
+              <c:y val="0.894241023817988"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4420,7 +4598,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1568728"/>
+        <c:crossAx val="99356174"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4428,7 +4606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1568728"/>
+        <c:axId val="99356174"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4471,7 +4649,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4343859"/>
+        <c:crossAx val="74032005"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4571,8 +4749,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.168487212830516"/>
-          <c:y val="0.0304505620961317"/>
+          <c:x val="0.168588520894746"/>
+          <c:y val="0.0304559539619301"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4590,10 +4768,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.149718248807976"/>
-          <c:y val="0.297424094892449"/>
-          <c:w val="0.831512787169484"/>
-          <c:h val="0.557316101619899"/>
+          <c:x val="0.149731229408705"/>
+          <c:y val="0.297299690128375"/>
+          <c:w val="0.831411479105254"/>
+          <c:h val="0.557237715803453"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -4950,11 +5128,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="40612313"/>
-        <c:axId val="43852538"/>
+        <c:axId val="30912007"/>
+        <c:axId val="16442101"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40612313"/>
+        <c:axId val="30912007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4987,7 +5165,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43852538"/>
+        <c:crossAx val="16442101"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4995,7 +5173,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43852538"/>
+        <c:axId val="16442101"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5038,7 +5216,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40612313"/>
+        <c:crossAx val="30912007"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5138,8 +5316,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.143621417076247"/>
-          <c:y val="0.0332808398950131"/>
+          <c:x val="0.143633911870895"/>
+          <c:y val="0.0332878294655046"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5157,10 +5335,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.150319690313601"/>
-          <c:y val="0.344356955380577"/>
-          <c:w val="0.830846853116437"/>
-          <c:h val="0.358320209973753"/>
+          <c:x val="0.150332767845491"/>
+          <c:y val="0.344219258636984"/>
+          <c:w val="0.830745138979512"/>
+          <c:h val="0.35818544576289"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -5661,11 +5839,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="50996382"/>
-        <c:axId val="59578185"/>
+        <c:axId val="3705132"/>
+        <c:axId val="32749003"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50996382"/>
+        <c:axId val="3705132"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5698,7 +5876,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59578185"/>
+        <c:crossAx val="32749003"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5706,7 +5884,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59578185"/>
+        <c:axId val="32749003"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5749,7 +5927,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50996382"/>
+        <c:crossAx val="3705132"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5849,8 +6027,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.272840661053945"/>
-          <c:y val="0.0305940946282462"/>
+          <c:x val="0.272775872054172"/>
+          <c:y val="0.0305995374488525"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5868,10 +6046,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.111853534678605"/>
-          <c:y val="0.298826040554963"/>
-          <c:w val="0.868991937280057"/>
-          <c:h val="0.555229455709712"/>
+          <c:x val="0.111863500690515"/>
+          <c:y val="0.298701298701299"/>
+          <c:w val="0.868891165857353"/>
+          <c:h val="0.555150329122932"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -6228,11 +6406,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="13327999"/>
-        <c:axId val="28463127"/>
+        <c:axId val="34686696"/>
+        <c:axId val="40633417"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="13327999"/>
+        <c:axId val="34686696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6265,7 +6443,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28463127"/>
+        <c:crossAx val="40633417"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6273,7 +6451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28463127"/>
+        <c:axId val="40633417"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6316,7 +6494,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13327999"/>
+        <c:crossAx val="34686696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6416,8 +6594,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.228414656267005"/>
-          <c:y val="0.033266659648384"/>
+          <c:x val="0.22843537414966"/>
+          <c:y val="0.033273665368011"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -6435,10 +6613,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.114184654453111"/>
-          <c:y val="0.348141909674703"/>
-          <c:w val="0.862098675857065"/>
-          <c:h val="0.353721444362565"/>
+          <c:x val="0.114195011337868"/>
+          <c:y val="0.348004633042013"/>
+          <c:w val="0.861995464852608"/>
+          <c:h val="0.353585342739813"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -6939,11 +7117,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="92107864"/>
-        <c:axId val="22327284"/>
+        <c:axId val="57334928"/>
+        <c:axId val="68904187"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92107864"/>
+        <c:axId val="57334928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6976,7 +7154,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22327284"/>
+        <c:crossAx val="68904187"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6984,7 +7162,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22327284"/>
+        <c:axId val="68904187"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7027,7 +7205,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92107864"/>
+        <c:crossAx val="57334928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7101,9 +7279,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1095120</xdr:colOff>
+      <xdr:colOff>1094400</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7112,7 +7290,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="740520" y="6705720"/>
-        <a:ext cx="9421200" cy="4952520"/>
+        <a:ext cx="9420480" cy="4951800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7131,9 +7309,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>285120</xdr:colOff>
+      <xdr:colOff>284400</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7142,7 +7320,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="10257120" y="6705720"/>
-        <a:ext cx="9719280" cy="4971600"/>
+        <a:ext cx="9718560" cy="4970880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7166,9 +7344,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>537840</xdr:colOff>
+      <xdr:colOff>537120</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>66240</xdr:rowOff>
+      <xdr:rowOff>65520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7177,7 +7355,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7561800" y="5972400"/>
-        <a:ext cx="9211680" cy="4618800"/>
+        <a:ext cx="9210960" cy="4618080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7196,9 +7374,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>509400</xdr:colOff>
+      <xdr:colOff>508680</xdr:colOff>
       <xdr:row>92</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7207,7 +7385,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7552440" y="10725120"/>
-        <a:ext cx="9192600" cy="4333680"/>
+        <a:ext cx="9191880" cy="4332960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7231,9 +7409,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1152000</xdr:colOff>
+      <xdr:colOff>1151280</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7242,7 +7420,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7780680" y="4162680"/>
-        <a:ext cx="8815680" cy="6076440"/>
+        <a:ext cx="8814960" cy="6075720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7266,9 +7444,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>418680</xdr:colOff>
+      <xdr:colOff>417960</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7277,7 +7455,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6636960" y="5886720"/>
-        <a:ext cx="8304840" cy="4066560"/>
+        <a:ext cx="8304120" cy="4065840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7296,9 +7474,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>390240</xdr:colOff>
+      <xdr:colOff>389520</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>28080</xdr:rowOff>
+      <xdr:rowOff>27360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7307,7 +7485,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6636960" y="10039320"/>
-        <a:ext cx="8276400" cy="3428640"/>
+        <a:ext cx="8275680" cy="3427920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7326,9 +7504,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>361440</xdr:colOff>
+      <xdr:colOff>360720</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7337,7 +7515,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15046920" y="5886720"/>
-        <a:ext cx="8081280" cy="4047480"/>
+        <a:ext cx="8080560" cy="4046760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7356,9 +7534,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>218520</xdr:colOff>
+      <xdr:colOff>217800</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7367,7 +7545,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15046920" y="10020240"/>
-        <a:ext cx="7938360" cy="3419280"/>
+        <a:ext cx="7937640" cy="3418560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7384,16 +7562,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>780120</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>209880</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>636840</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>284400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>43920</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>713160</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7401,8 +7579,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3218400" y="4550760"/>
-        <a:ext cx="5766480" cy="3231000"/>
+        <a:off x="4885560" y="3338280"/>
+        <a:ext cx="5766120" cy="4168800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9687,7 +9865,7 @@
   </sheetPr>
   <dimension ref="B7:J31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -10087,7 +10265,7 @@
   </sheetPr>
   <dimension ref="A6:P89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q58" activeCellId="0" sqref="Q58"/>
     </sheetView>
   </sheetViews>
@@ -10160,16 +10338,16 @@
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="26"/>
       <c r="C9" s="25"/>
-      <c r="D9" s="0"/>
-      <c r="E9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
       <c r="F9" s="26"/>
       <c r="G9" s="25"/>
-      <c r="H9" s="0"/>
-      <c r="I9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="26"/>
       <c r="K9" s="25"/>
-      <c r="L9" s="0"/>
-      <c r="M9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="47"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
@@ -10407,7 +10585,7 @@
       <c r="H25" s="13"/>
       <c r="I25" s="3"/>
       <c r="J25" s="33"/>
-      <c r="K25" s="47"/>
+      <c r="K25" s="48"/>
       <c r="L25" s="13"/>
       <c r="M25" s="3"/>
     </row>
@@ -10572,19 +10750,19 @@
       <c r="B34" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="48"/>
+      <c r="C34" s="49"/>
       <c r="D34" s="21"/>
       <c r="E34" s="11"/>
       <c r="F34" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="G34" s="48"/>
+      <c r="G34" s="49"/>
       <c r="H34" s="21"/>
       <c r="I34" s="11"/>
       <c r="J34" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="K34" s="48"/>
+      <c r="K34" s="49"/>
       <c r="L34" s="21"/>
       <c r="M34" s="11"/>
     </row>
@@ -10687,7 +10865,7 @@
       <c r="B41" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="49" t="n">
+      <c r="C41" s="50" t="n">
         <v>0</v>
       </c>
       <c r="D41" s="4" t="n">
@@ -10925,7 +11103,7 @@
       <c r="B57" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="49" t="n">
+      <c r="C57" s="50" t="n">
         <v>0</v>
       </c>
       <c r="D57" s="4" t="n">
@@ -10940,7 +11118,7 @@
       <c r="B58" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C58" s="49" t="n">
+      <c r="C58" s="50" t="n">
         <v>0</v>
       </c>
       <c r="D58" s="4" t="n">
@@ -10955,7 +11133,7 @@
       <c r="B59" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C59" s="49" t="n">
+      <c r="C59" s="50" t="n">
         <v>0</v>
       </c>
       <c r="D59" s="4" t="n">
@@ -11043,7 +11221,7 @@
       <c r="B65" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="49" t="n">
+      <c r="C65" s="50" t="n">
         <v>0</v>
       </c>
       <c r="D65" s="4" t="n">
@@ -11281,7 +11459,7 @@
       <c r="B81" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C81" s="49" t="n">
+      <c r="C81" s="50" t="n">
         <v>0</v>
       </c>
       <c r="D81" s="4" t="n">
@@ -11296,7 +11474,7 @@
       <c r="B82" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C82" s="49" t="n">
+      <c r="C82" s="50" t="n">
         <v>0</v>
       </c>
       <c r="D82" s="4" t="n">
@@ -11311,7 +11489,7 @@
       <c r="B83" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C83" s="49" t="n">
+      <c r="C83" s="50" t="n">
         <v>0</v>
       </c>
       <c r="D83" s="4" t="n">
@@ -11413,185 +11591,241 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.98"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="44" t="s">
-        <v>41</v>
-      </c>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="44"/>
       <c r="B1" s="4" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <f aca="false">B1/$B1</f>
-        <v>1</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <f aca="false">C1/$B1</f>
-        <v>0.0089119170984456</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="C2" s="51" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="D2" s="51" t="n">
+        <v>0.527</v>
+      </c>
+      <c r="E2" s="46" t="n">
         <f aca="false">B2/$B2</f>
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="F2" s="46" t="n">
         <f aca="false">C2/$B2</f>
-        <v>0.037</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.00639032815198618</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">D2/B2</f>
+        <v>0.00910189982728843</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">B3/$B3</f>
+        <v>72</v>
+      </c>
+      <c r="B3" s="52" t="n">
+        <v>0.00275</v>
+      </c>
+      <c r="C3" s="51" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D3" s="51" t="n">
+        <v>0.0329</v>
+      </c>
+      <c r="E3" s="46" t="n">
+        <f aca="false">B3/$C3</f>
+        <v>0.1375</v>
+      </c>
+      <c r="F3" s="46" t="n">
+        <f aca="false">C3/$C3</f>
         <v>1</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <f aca="false">C3/$B3</f>
-        <v>0.0150333333333333</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="0" t="n">
+        <f aca="false">D3/C3</f>
+        <v>1.645</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">B4/$B4</f>
+        <v>73</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>363</v>
+      </c>
+      <c r="C4" s="51" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="D4" s="51" t="n">
+        <v>49.426</v>
+      </c>
+      <c r="E4" s="46" t="n">
+        <f aca="false">B4/B4</f>
         <v>1</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <f aca="false">C4/$B4</f>
-        <v>0.0415277777777778</v>
+      <c r="F4" s="46" t="n">
+        <f aca="false">C4/B4</f>
+        <v>0.093939393939394</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">D4/B4</f>
+        <v>0.136159779614325</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="44" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="C5" s="51" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="D5" s="51" t="n">
+        <v>0.0235</v>
+      </c>
+      <c r="E5" s="46" t="n">
         <f aca="false">B5/$B5</f>
         <v>1</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="F5" s="46" t="n">
         <f aca="false">C5/$B5</f>
-        <v>0.0246666666666667</v>
+        <v>0.283333333333333</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">D5/B5</f>
+        <v>0.391666666666667</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="44" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="0" t="n">
+      <c r="C6" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="51" t="n">
+        <v>0.562</v>
+      </c>
+      <c r="E6" s="46" t="n">
         <f aca="false">B6/$B6</f>
         <v>1</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="F6" s="46" t="n">
         <f aca="false">C6/$B6</f>
-        <v>0.0111785714285714</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="44"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>0.0089119170984456</v>
-      </c>
+        <v>0.0135714285714286</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">D6/B6</f>
+        <v>0.0200714285714286</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
     </row>
     <row r="9" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B9" s="53" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>0.037</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="52" t="n">
+        <v>0.00639032815198618</v>
+      </c>
+      <c r="D9" s="52" t="n">
+        <v>0.00910189982728843</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B10" s="54" t="n">
+        <v>0.1375</v>
+      </c>
+      <c r="C10" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="0" t="n">
-        <v>0.0150333333333333</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="55" t="n">
+        <v>1.645</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="B11" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <v>0.0111785714285714</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="44"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C11" s="55" t="n">
+        <v>0.093939393939394</v>
+      </c>
+      <c r="D11" s="55" t="n">
+        <v>0.136159779614325</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="55" t="n">
+        <v>0.283333333333333</v>
+      </c>
+      <c r="D12" s="55" t="n">
+        <v>0.391666666666667</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="55" t="n">
+        <v>0.0135714285714286</v>
+      </c>
+      <c r="D13" s="55" t="n">
+        <v>0.0200714285714286</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="44"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>